<commit_message>
case9. Num scenarios updated.
</commit_message>
<xml_diff>
--- a/data/CS5/case9/case9_2025.xlsx
+++ b/data/CS5/case9/case9_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\case9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12037FC0-E17E-48DA-845E-760A4278B200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B66961-2B5A-4043-B8BB-592FC2C700D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38145" yWindow="-11715" windowWidth="28800" windowHeight="15285" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34200" yWindow="-8880" windowWidth="28800" windowHeight="15285" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -4401,7 +4401,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4417,39 +4417,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="1">
+        <f>1/$B$1</f>
         <v>1</v>
       </c>
       <c r="D1" s="1">
-        <f t="shared" ref="D1:E1" si="0">1/3</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" ref="D1:K1" si="0">1/$B$1</f>
+        <v>1</v>
       </c>
       <c r="E1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1">
-        <f t="shared" ref="F1:K1" si="1">1/9</f>
-        <v>0.1111111111111111</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="G1" s="1">
-        <f t="shared" si="1"/>
-        <v>0.1111111111111111</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H1" s="1">
-        <f t="shared" si="1"/>
-        <v>0.1111111111111111</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I1" s="1">
-        <f t="shared" si="1"/>
-        <v>0.1111111111111111</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J1" s="1">
-        <f t="shared" si="1"/>
-        <v>0.1111111111111111</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="K1" s="1">
-        <f t="shared" si="1"/>
-        <v>0.1111111111111111</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
case9. Num scenarios increased
</commit_message>
<xml_diff>
--- a/data/CS5/case9/case9_2025.xlsx
+++ b/data/CS5/case9/case9_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\case9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802628D9-BF1C-4E09-AA93-D2042B92CA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D60D001-2777-4CA3-8CDC-961FABE3E04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31575" yWindow="-11220" windowWidth="17280" windowHeight="9960" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="9960" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -4414,43 +4414,43 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="D1" s="1">
         <f t="shared" ref="D1:K1" si="0">1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="E1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="G1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="H1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="I1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="J1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Test. Num scenarios increased.
</commit_message>
<xml_diff>
--- a/data/CS5/case9/case9_2025.xlsx
+++ b/data/CS5/case9/case9_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\case9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C137B83-D8AA-4323-80C9-22C59C092136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8348CED-5FB9-449D-B28A-7BE6FD030DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4414,43 +4414,43 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="D1" s="1">
         <f t="shared" ref="D1:K1" si="0">1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="E1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="G1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="H1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="I1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="J1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
case_9. Num scenarios updated.
</commit_message>
<xml_diff>
--- a/data/CS5/case9/case9_2025.xlsx
+++ b/data/CS5/case9/case9_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\case9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8348CED-5FB9-449D-B28A-7BE6FD030DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62D7973-94D5-4948-8FA7-4059490E0F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4414,43 +4414,43 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
         <f t="shared" ref="D1:K1" si="0">1/$B$1</f>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E1" s="1">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F1" s="1">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G1" s="1">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H1" s="1">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I1" s="1">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J1" s="1">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K1" s="1">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Test. 5 years, All scenarios
</commit_message>
<xml_diff>
--- a/data/CS5/case9/case9_2025.xlsx
+++ b/data/CS5/case9/case9_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\case9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E1F30B-0FB2-48D6-8E89-D43D6E3DD368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFB0B30-8E13-4B50-B7E3-55E721FAB8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-14400" windowWidth="38640" windowHeight="21120" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -4414,43 +4414,43 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="D1" s="1">
         <f t="shared" ref="D1:K1" si="0">1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="E1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="G1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="H1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="I1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="J1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K1" s="1">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Test. 5 years, All scenarios DN. 3 TN
</commit_message>
<xml_diff>
--- a/data/CS5/case9/case9_2025.xlsx
+++ b/data/CS5/case9/case9_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\case9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFB0B30-8E13-4B50-B7E3-55E721FAB8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6109A0A4-1AEE-4B59-98CA-C46C24CAC184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4414,43 +4414,43 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
         <f t="shared" ref="D1:K1" si="0">1/$B$1</f>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E1" s="1">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F1" s="1">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G1" s="1">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H1" s="1">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I1" s="1">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J1" s="1">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K1" s="1">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>